<commit_message>
read the output file and keep updating it.
</commit_message>
<xml_diff>
--- a/robodogbatch/batch.xlsx
+++ b/robodogbatch/batch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\robodog\robodogbatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA98E045-CE37-4ED0-B5F6-D1E00D6E5115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1774E8-205B-4EA0-9B53-877EB9F90C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{D4159D3E-8F98-4802-931F-BFE7F7EE349F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>knowledge</t>
   </si>
@@ -59,84 +59,22 @@
     <t>title</t>
   </si>
   <si>
-    <t>from os import name
-import pandas as pd
-import openpyxl
-import openai
-import logging
-logging.basicConfig(filename='output.log', level=logging.INFO,
-                    format='%(asctime)s - %(levelname)s - %(message)s')
-class Model:
-    def init(self, title, group, knowledge, question, output, m):
-        self.title = title
-        self.group = group
-        self.question = question
-        self.m = m
-        self.knowledge = knowledge
-        self.output = output
-def processmodelswith_openai(models, token):
-    openai.api_key = token
-    for model in models:
-        try:
-            logging.info(f"{model.title}: {model.output}")
-            response = openai.ChatCompletion.create(
-                model=model.m,
-                messages=[
-                    {"role": "system", "content": "You are a helpful assistant."},
-                    {"role": "user", "content": f"Context: {model.knowledge}\nQuestion: {model.question}"}
-                ]
-            )
-            model.output = response.choices[0].message['content'].strip()
-            logging.info(f"{model.title}: {model.output}")
-        except Exception as e:
-            logging.error(f"OpenAI API error for {model.title}: {e}")
-def readexcel(filepath, group_filter):
-    try:
-        logging.info("Reading file " + filepath + " with group " + group_filter)
-        df = pd.read_excel(filepath)
-        models = []
-        for _, row in df.iterrows():
-            title = row.get('title')
-            group = row.get('group')
-            question = row.get('question')
-            m = row.get('model')
-            knowledge = row.get('knowledge')
-            output = row.get('output')
-            if title and group and knowledge and pd.notna(group) and group == group_filter:
-                model = Model(title, group, knowledge, question, output, m)
-                models.append(model)
-                logging.info(f"Model: {m} Title: {title}, Group: {group}, Knowledge: {knowledge}, Question: {question}, Output: {output}")
-            else:
-                logging.debug("Missing or unmatched data in row: " + str(row))
-        return models
-    except FileNotFoundError:
-        logging.error("File not found: " + filepath)
-        return []
-    except Exception as e:
-        logging.error("Error: " + str(e))
-        return []
-def main(filename, group, token):
-    logging.info(f"Processing file: {filename} for group: {group}")
-    models = readexcel(filename, group)
-    processmodelswith_openai(models, token)
-    for model in models:
-        print(model.title, model.group, model.knowledge, model.output)
-import sys
-print("start")
-logging.info("Batch processing started")
-if len(sys.argv) &gt; 3:
-    filename = sys.argv[1]
-    group = sys.argv[2]
-    token = sys.argv[3]
-    main(filename, group, token)
-else:
-    print("Provide Excel file, group, and token.")</t>
-  </si>
-  <si>
-    <t>convert to powershell</t>
-  </si>
-  <si>
     <t>outputfile</t>
+  </si>
+  <si>
+    <t>&lt;Measure name="Total Sales" Aggregator="Sum" Column="FactTable.SalesAmount" /&gt;</t>
+  </si>
+  <si>
+    <t>g1 total sales sum measure</t>
+  </si>
+  <si>
+    <t>g1 total sales avg measure</t>
+  </si>
+  <si>
+    <t>&lt;Measure name="Total Sales" Aggregator="Avg" Column="FactTable.SalesAmount" /&gt;</t>
+  </si>
+  <si>
+    <t>convert ssas measure to a sql server function.  Just give me the function code. Ne comments or explanation</t>
   </si>
 </sst>
 </file>
@@ -177,11 +115,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -202,7 +137,7 @@
         <name val="Congenial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -220,7 +155,7 @@
         <name val="Congenial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -235,7 +170,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -249,7 +184,7 @@
         <name val="Congenial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -263,7 +198,7 @@
         <name val="Congenial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -277,7 +212,7 @@
         <name val="Congenial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -291,7 +226,7 @@
         <name val="Congenial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -305,7 +240,7 @@
         <name val="Congenial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -657,21 +592,21 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="15.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="55" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="1" customWidth="1"/>
+    <col min="4" max="4" width="50.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.109375" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -688,253 +623,268 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
-        <v>g1-convert to powershell.sql</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>g1-g1 total sales sum measure.sql</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F3" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
-        <v>-.sql</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>g1-g1 total sales avg measure.sql</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F4" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F5" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F6" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F7" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F8" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F9" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F10" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F11" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F12" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F13" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F14" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F15" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F16" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F17" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F18" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F19" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F20" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F21" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F22" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F23" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F24" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F25" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F26" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F27" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F28" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F29" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F30" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F31" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F32" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F33" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F34" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F35" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F36" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F37" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F38" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F39" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F40" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>

</xml_diff>

<commit_message>
updates to the excel template
</commit_message>
<xml_diff>
--- a/robodogbatch/batch.xlsx
+++ b/robodogbatch/batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\robodog\robodogbatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1774E8-205B-4EA0-9B53-877EB9F90C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD089E9-8752-424C-8344-51C238567544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{D4159D3E-8F98-4802-931F-BFE7F7EE349F}"/>
+    <workbookView xWindow="-180" yWindow="1572" windowWidth="29652" windowHeight="15912" xr2:uid="{D4159D3E-8F98-4802-931F-BFE7F7EE349F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>knowledge</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>convert ssas measure to a sql server function.  Just give me the function code. Ne comments or explanation</t>
+  </si>
+  <si>
+    <t>I want to mock the fact table but I want best performance. Will this be a hit to performance?</t>
   </si>
 </sst>
 </file>
@@ -592,7 +595,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -601,12 +604,12 @@
     <col min="2" max="2" width="24.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" customWidth="1"/>
     <col min="4" max="4" width="50.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.21875" style="1" customWidth="1"/>
     <col min="6" max="6" width="32.109375" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -626,7 +629,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -640,14 +643,14 @@
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>g1-g1 total sales sum measure.sql</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -668,223 +671,223 @@
         <v>g1-g1 total sales avg measure.sql</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F4" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F5" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F6" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F7" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F8" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F9" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F10" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F11" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F12" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F13" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F14" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F15" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F16" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="17" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F17" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="18" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F18" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="19" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F19" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="20" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F20" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="21" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F21" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="22" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F22" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="23" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F23" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="24" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F24" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="25" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F25" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="26" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F26" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="27" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F27" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="28" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F28" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="29" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F29" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="30" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F30" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="31" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F31" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="32" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F32" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="33" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F33" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="34" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F34" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="35" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F35" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="36" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F36" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="37" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F37" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="38" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F38" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="39" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F39" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>
       </c>
     </row>
-    <row r="40" spans="6:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F40" s="1" t="str">
         <f>Table1[[#This Row],[group]]&amp;"-"&amp;Table1[[#This Row],[title]]&amp;".sql"</f>
         <v>-.sql</v>

</xml_diff>